<commit_message>
Added color coding for deprecation
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v7 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v7 draft.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$K$76</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -650,12 +650,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -679,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -706,6 +712,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1109,26 +1124,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.36328125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="103.08984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="103.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.36328125" style="4"/>
-    <col min="11" max="11" width="64.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.36328125" style="4"/>
+    <col min="5" max="5" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="4"/>
+    <col min="11" max="11" width="64.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="29">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="45">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -1163,7 +1178,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="43.5">
+    <row r="2" spans="1:11" ht="45">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1212,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.5">
+    <row r="3" spans="1:11" ht="45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1231,7 +1246,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="43.5">
+    <row r="4" spans="1:11" ht="45">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1265,7 +1280,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29">
+    <row r="5" spans="1:11" ht="45">
       <c r="A5" s="4" t="s">
         <v>125</v>
       </c>
@@ -1299,7 +1314,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.5">
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="4" t="s">
         <v>128</v>
       </c>
@@ -1333,7 +1348,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="43.5">
+    <row r="7" spans="1:11" ht="45">
       <c r="A7" s="4" t="s">
         <v>128</v>
       </c>
@@ -1367,38 +1382,38 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="E8" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29">
+    <row r="9" spans="1:11" ht="30">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29">
+    <row r="10" spans="1:11" ht="45">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -1469,38 +1484,38 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="6">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="D11" s="12">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
         <v>2</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K11" s="4" t="s">
+      <c r="J11" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29">
+    <row r="12" spans="1:11" ht="30">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1534,38 +1549,38 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="29">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="E13" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="10">
         <v>2</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K13" s="4" t="s">
+      <c r="J13" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="29">
+    <row r="14" spans="1:11" ht="30">
       <c r="A14" s="2" t="s">
         <v>126</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29">
+    <row r="15" spans="1:11" ht="45">
       <c r="A15" s="2" t="s">
         <v>127</v>
       </c>
@@ -1633,7 +1648,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29">
+    <row r="16" spans="1:11" ht="30">
       <c r="A16" s="2" t="s">
         <v>126</v>
       </c>
@@ -1667,255 +1682,255 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="29">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A17" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I17" s="4">
+      <c r="E17" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="10">
         <v>2</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K17" s="4" t="s">
+      <c r="J17" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="29">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A18" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I18" s="4">
+      <c r="E18" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="10">
         <v>2</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K18" s="4" t="s">
+      <c r="J18" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:11" s="10" customFormat="1" ht="30">
+      <c r="A19" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="4" t="s">
+      <c r="E19" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="43.5">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A20" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="E20" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K20" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="43.5">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A21" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K21" s="4" t="s">
+      <c r="E21" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:11" s="10" customFormat="1" ht="30">
+      <c r="A22" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K22" s="4" t="s">
+      <c r="E22" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="29">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A23" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K23" s="4" t="s">
+      <c r="E23" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I23" s="10">
+        <v>1</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K23" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="29">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:11" s="10" customFormat="1" ht="30">
+      <c r="A24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I24" s="4">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K24" s="4" t="s">
+      <c r="E24" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="10">
+        <v>1</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K24" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="43.5">
+    <row r="25" spans="1:11" ht="45">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1946,7 +1961,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43.5">
+    <row r="26" spans="1:11" ht="45">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1974,38 +1989,38 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="29">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A27" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K27" s="4" t="s">
+      <c r="E27" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="29">
+    <row r="28" spans="1:11" ht="45">
       <c r="A28" s="4" t="s">
         <v>120</v>
       </c>
@@ -2041,100 +2056,100 @@
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="43.5">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A29" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="6">
-        <v>3</v>
-      </c>
-      <c r="E29" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K29" s="4" t="s">
+      <c r="D29" s="12">
+        <v>3</v>
+      </c>
+      <c r="E29" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K29" s="10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="43.5">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A30" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I30" s="4">
-        <v>1</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" s="4" t="s">
+      <c r="E30" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>1</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K30" s="10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="43.5">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:11" s="10" customFormat="1" ht="45">
+      <c r="A31" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I31" s="4">
-        <v>1</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K31" s="4" t="s">
+      <c r="E31" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="10">
+        <v>1</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K31" s="10" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="29">
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="4" t="s">
         <v>107</v>
       </c>
@@ -2165,7 +2180,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="29">
+    <row r="33" spans="1:11" ht="30">
       <c r="A33" s="4" t="s">
         <v>108</v>
       </c>
@@ -2196,7 +2211,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="43.5">
+    <row r="34" spans="1:11" ht="45">
       <c r="A34" s="4" t="s">
         <v>118</v>
       </c>
@@ -2224,7 +2239,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="43.5">
+    <row r="35" spans="1:11" ht="45">
       <c r="A35" s="4" t="s">
         <v>153</v>
       </c>
@@ -2252,7 +2267,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="29">
+    <row r="36" spans="1:11" ht="30">
       <c r="A36" s="4" t="s">
         <v>109</v>
       </c>
@@ -2283,7 +2298,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="43.5">
+    <row r="37" spans="1:11" ht="45">
       <c r="A37" s="4" t="s">
         <v>117</v>
       </c>
@@ -2314,7 +2329,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="43.5">
+    <row r="38" spans="1:11" ht="45">
       <c r="A38" s="4" t="s">
         <v>116</v>
       </c>
@@ -2345,7 +2360,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="43.5">
+    <row r="39" spans="1:11" ht="45">
       <c r="A39" s="4" t="s">
         <v>115</v>
       </c>
@@ -2376,7 +2391,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="43.5">
+    <row r="40" spans="1:11" ht="45">
       <c r="A40" s="4" t="s">
         <v>114</v>
       </c>
@@ -2407,7 +2422,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="43.5">
+    <row r="41" spans="1:11" ht="45">
       <c r="A41" s="4" t="s">
         <v>112</v>
       </c>
@@ -2438,7 +2453,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="29">
+    <row r="42" spans="1:11" ht="45">
       <c r="A42" s="4" t="s">
         <v>113</v>
       </c>
@@ -2469,7 +2484,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="29">
+    <row r="43" spans="1:11" ht="30">
       <c r="A43" s="4" t="s">
         <v>129</v>
       </c>
@@ -2499,7 +2514,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="29">
+    <row r="44" spans="1:11" ht="30">
       <c r="A44" s="4" t="s">
         <v>130</v>
       </c>
@@ -2529,7 +2544,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="29">
+    <row r="45" spans="1:11" ht="30">
       <c r="A45" s="4" t="s">
         <v>131</v>
       </c>
@@ -2615,7 +2630,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="29">
+    <row r="48" spans="1:11" ht="30">
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
@@ -2643,7 +2658,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="29">
+    <row r="49" spans="1:11" ht="30">
       <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
@@ -2671,38 +2686,38 @@
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="29">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:11" s="10" customFormat="1" ht="30">
+      <c r="A50" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="4" t="s">
+      <c r="B50" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="10">
         <v>4</v>
       </c>
-      <c r="E50" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H50" s="4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="I50" s="4">
-        <v>1</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K50" s="4" t="s">
+      <c r="E50" s="10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="I50" s="10">
+        <v>1</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K50" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="29">
+    <row r="51" spans="1:11" ht="45">
       <c r="A51" s="4" t="s">
         <v>84</v>
       </c>
@@ -2733,7 +2748,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="29">
+    <row r="52" spans="1:11" ht="30">
       <c r="A52" s="4" t="s">
         <v>85</v>
       </c>
@@ -2764,7 +2779,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="29">
+    <row r="53" spans="1:11" ht="30">
       <c r="A53" s="4" t="s">
         <v>86</v>
       </c>
@@ -2795,7 +2810,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="29">
+    <row r="54" spans="1:11" ht="30">
       <c r="A54" s="4" t="s">
         <v>87</v>
       </c>
@@ -2826,7 +2841,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" ht="30">
       <c r="A55" s="4" t="s">
         <v>88</v>
       </c>
@@ -2857,7 +2872,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="29">
+    <row r="56" spans="1:11" ht="30">
       <c r="A56" s="4" t="s">
         <v>89</v>
       </c>
@@ -2888,7 +2903,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="29">
+    <row r="57" spans="1:11" ht="30">
       <c r="A57" s="4" t="s">
         <v>90</v>
       </c>
@@ -2919,7 +2934,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="29">
+    <row r="58" spans="1:11" ht="30">
       <c r="A58" s="4" t="s">
         <v>91</v>
       </c>
@@ -2950,7 +2965,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="29">
+    <row r="59" spans="1:11" ht="30">
       <c r="A59" s="4" t="s">
         <v>92</v>
       </c>
@@ -2981,7 +2996,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="29">
+    <row r="60" spans="1:11" ht="30">
       <c r="A60" s="4" t="s">
         <v>93</v>
       </c>
@@ -3009,7 +3024,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="29">
+    <row r="61" spans="1:11" ht="30">
       <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
@@ -3037,7 +3052,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="29">
+    <row r="62" spans="1:11" ht="30">
       <c r="A62" s="4" t="s">
         <v>97</v>
       </c>
@@ -3068,7 +3083,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="29">
+    <row r="63" spans="1:11" ht="45">
       <c r="A63" s="4" t="s">
         <v>98</v>
       </c>
@@ -3105,7 +3120,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="29">
+    <row r="64" spans="1:11" ht="45">
       <c r="A64" s="4" t="s">
         <v>98</v>
       </c>
@@ -3136,7 +3151,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="29">
+    <row r="65" spans="1:11" ht="30">
       <c r="A65" s="4" t="s">
         <v>101</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="29">
+    <row r="66" spans="1:11" ht="30">
       <c r="A66" s="4" t="s">
         <v>102</v>
       </c>
@@ -3192,7 +3207,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="29">
+    <row r="67" spans="1:11" ht="30">
       <c r="A67" s="4" t="s">
         <v>103</v>
       </c>
@@ -3220,7 +3235,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="29">
+    <row r="68" spans="1:11" ht="30">
       <c r="A68" s="4" t="s">
         <v>132</v>
       </c>
@@ -3248,7 +3263,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="43.5">
+    <row r="69" spans="1:11" ht="45">
       <c r="A69" s="4" t="s">
         <v>133</v>
       </c>
@@ -3276,7 +3291,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="29">
+    <row r="70" spans="1:11" ht="30">
       <c r="A70" s="4" t="s">
         <v>137</v>
       </c>
@@ -3304,7 +3319,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="29">
+    <row r="71" spans="1:11" ht="45">
       <c r="A71" s="9" t="s">
         <v>145</v>
       </c>
@@ -3335,7 +3350,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="29">
+    <row r="72" spans="1:11" ht="45">
       <c r="A72" s="9" t="s">
         <v>144</v>
       </c>
@@ -3366,7 +3381,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="29">
+    <row r="73" spans="1:11" ht="45">
       <c r="A73" s="4" t="s">
         <v>143</v>
       </c>
@@ -3394,7 +3409,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="43.5">
+    <row r="74" spans="1:11" ht="45">
       <c r="A74" s="4" t="s">
         <v>146</v>
       </c>
@@ -3422,7 +3437,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="43.5">
+    <row r="75" spans="1:11" ht="45">
       <c r="A75" s="4" t="s">
         <v>190</v>
       </c>
@@ -3450,7 +3465,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="43.5">
+    <row r="76" spans="1:11" ht="45">
       <c r="A76" s="4" t="s">
         <v>193</v>
       </c>
@@ -3479,7 +3494,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K74"/>
+  <autoFilter ref="A1:K76"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed errors in document types
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Document types v7 draft.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Document types v7 draft.xlsx
@@ -631,9 +631,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.3::2.1</t>
   </si>
   <si>
-    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.3:16B</t>
-  </si>
-  <si>
     <t>TICC-117: deprecate per 2021-01-01</t>
   </si>
   <si>
@@ -652,9 +649,6 @@
     <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.0::2.1</t>
   </si>
   <si>
-    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.0:16B</t>
-  </si>
-  <si>
     <t>XRechnung UBL Invoice V1.3 Extension</t>
   </si>
   <si>
@@ -704,6 +698,12 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:fdc:peppol.eu:poacc:trns:order_response:3:extended:urn:fdc:anskaffelser.no:2019:ehf:spec:3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_1.3::16B</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xoev-de:kosit:standard:xrechnung_2.0::16B</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1200,8 @@
   <dimension ref="A1:K90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -3293,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H65" s="3" t="b">
         <f>FALSE</f>
@@ -3324,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H66" s="3" t="b">
         <f>FALSE</f>
@@ -3355,7 +3355,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H67" s="3" t="b">
         <f>FALSE</f>
@@ -3690,7 +3690,7 @@
         <v>60</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="D79" s="3">
         <v>7</v>
@@ -3712,13 +3712,13 @@
     </row>
     <row r="80" spans="1:11" ht="30">
       <c r="A80" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D80" s="3">
         <v>7</v>
@@ -3740,13 +3740,13 @@
     </row>
     <row r="81" spans="1:11" ht="30">
       <c r="A81" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D81" s="3">
         <v>7</v>
@@ -3768,13 +3768,13 @@
     </row>
     <row r="82" spans="1:11" ht="30">
       <c r="A82" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D82" s="3">
         <v>7</v>
@@ -3796,13 +3796,13 @@
     </row>
     <row r="83" spans="1:11" ht="30">
       <c r="A83" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D83" s="3">
         <v>7</v>
@@ -3824,13 +3824,13 @@
     </row>
     <row r="84" spans="1:11" ht="45">
       <c r="A84" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D84" s="3">
         <v>7</v>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="85" spans="1:11" ht="45">
       <c r="A85" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D85" s="3">
         <v>7</v>
@@ -3880,13 +3880,13 @@
     </row>
     <row r="86" spans="1:11" ht="45">
       <c r="A86" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D86" s="3">
         <v>7</v>
@@ -3908,13 +3908,13 @@
     </row>
     <row r="87" spans="1:11" ht="30">
       <c r="A87" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D87" s="3">
         <v>7</v>
@@ -3931,18 +3931,18 @@
         <v>142</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="30">
       <c r="A88" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D88" s="3">
         <v>7</v>
@@ -3959,18 +3959,18 @@
         <v>142</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="30">
       <c r="A89" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D89" s="3">
         <v>7</v>
@@ -3987,18 +3987,18 @@
         <v>142</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="45">
       <c r="A90" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D90" s="3">
         <v>7</v>
@@ -4015,7 +4015,7 @@
         <v>142</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>